<commit_message>
fix typo in datamodel field label
</commit_message>
<xml_diff>
--- a/molgenis-data-model/mosaic_model.xlsx
+++ b/molgenis-data-model/mosaic_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Code/molgenis-app-mosaic-calculator/molgenis-data-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58B3F1-142F-C644-BC28-6E52FE0003FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F135E2-A1F8-0F4A-89D9-5A7904FB929C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="15220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>event data</t>
   </si>
   <si>
-    <t>snp BAF dat</t>
+    <t>snp BAF data</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +508,8 @@
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="24.83203125" customWidth="1"/>
-    <col min="8" max="8" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Stop storing result file id with experiment data
- update cleanup script, data cleanup is now done using filter with '.mosaic.pdf'
- remove resultId attribute form model entity
- remove code to store result fileId ( + remove tests)
- update setup readme with note on file extension
</commit_message>
<xml_diff>
--- a/molgenis-data-model/mosaic_model.xlsx
+++ b/molgenis-data-model/mosaic_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Code/molgenis-app-mosaic-calculator/molgenis-data-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F135E2-A1F8-0F4A-89D9-5A7904FB929C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD331AD5-D323-6F4C-85E2-D2EE173BCB42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="15220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -102,18 +102,6 @@
   </si>
   <si>
     <t>mosaic_exp_data</t>
-  </si>
-  <si>
-    <t>resultFileId</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>result file id</t>
-  </si>
-  <si>
-    <t>The entity id of the result file</t>
   </si>
   <si>
     <t>event data</t>
@@ -497,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -615,30 +603,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>